<commit_message>
thêm api add chitietphancong excel và cập nhật lại file excel
</commit_message>
<xml_diff>
--- a/Tài liệu/chitietphancong_thuocbomon_CNTT.xlsx
+++ b/Tài liệu/chitietphancong_thuocbomon_CNTT.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\NghienCuuKhoaHoc\Tài liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EBD6816-6E36-4B41-A052-E8B1E330E9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{82CE0BEE-9960-4F02-9FA2-CE0238C9E553}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="13905"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -267,7 +266,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -366,7 +365,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -677,24 +676,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5685171-40AF-4BB9-B2E5-AADD1356981F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.90625" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.6328125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -711,7 +710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -728,7 +727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -745,7 +744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -762,7 +761,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -779,7 +778,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -796,7 +795,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -813,7 +812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -830,7 +829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -847,7 +846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -864,7 +863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -881,7 +880,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -898,7 +897,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
@@ -915,7 +914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
@@ -932,7 +931,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
@@ -949,7 +948,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
@@ -966,7 +965,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
@@ -983,7 +982,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
@@ -1000,7 +999,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>28</v>
       </c>
@@ -1017,7 +1016,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>28</v>
       </c>
@@ -1034,7 +1033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>31</v>
       </c>
@@ -1051,7 +1050,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>31</v>
       </c>
@@ -1068,7 +1067,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>31</v>
       </c>
@@ -1085,7 +1084,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>31</v>
       </c>
@@ -1102,7 +1101,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
@@ -1119,7 +1118,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>35</v>
       </c>
@@ -1136,7 +1135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>35</v>
       </c>
@@ -1153,7 +1152,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>35</v>
       </c>
@@ -1170,7 +1169,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
@@ -1187,7 +1186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>39</v>
       </c>
@@ -1204,7 +1203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -1221,7 +1220,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>39</v>
       </c>
@@ -1238,7 +1237,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>39</v>
       </c>
@@ -1255,7 +1254,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>42</v>
       </c>
@@ -1272,7 +1271,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
@@ -1289,7 +1288,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -1306,7 +1305,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>42</v>
       </c>
@@ -1323,7 +1322,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
@@ -1340,7 +1339,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="57" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>44</v>
       </c>
@@ -1357,7 +1356,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="57" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -1374,7 +1373,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
@@ -1391,7 +1390,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>44</v>
       </c>
@@ -1408,7 +1407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
@@ -1425,7 +1424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>47</v>
       </c>
@@ -1442,7 +1441,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>47</v>
       </c>
@@ -1459,7 +1458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>49</v>
       </c>
@@ -1476,7 +1475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>49</v>
       </c>
@@ -1493,7 +1492,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
@@ -1510,7 +1509,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>49</v>
       </c>
@@ -1527,7 +1526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
@@ -1544,7 +1543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
@@ -1561,7 +1560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>52</v>
       </c>
@@ -1578,7 +1577,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
@@ -1595,7 +1594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
@@ -1612,7 +1611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
@@ -1629,7 +1628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>52</v>
       </c>
@@ -1646,7 +1645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>52</v>
       </c>
@@ -1663,7 +1662,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
@@ -1680,7 +1679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
@@ -1697,7 +1696,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>60</v>
       </c>
@@ -1714,7 +1713,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
@@ -1731,7 +1730,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
@@ -1748,7 +1747,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>60</v>
       </c>
@@ -1765,7 +1764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>60</v>
       </c>
@@ -1782,7 +1781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>62</v>
       </c>
@@ -1799,7 +1798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>62</v>
       </c>
@@ -1816,7 +1815,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>62</v>
       </c>
@@ -1833,7 +1832,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>65</v>
       </c>
@@ -1850,7 +1849,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>65</v>
       </c>
@@ -1867,7 +1866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>65</v>
       </c>
@@ -1884,7 +1883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>66</v>
       </c>
@@ -1901,7 +1900,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>66</v>
       </c>
@@ -1918,7 +1917,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>67</v>
       </c>
@@ -1935,7 +1934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>67</v>
       </c>
@@ -1952,7 +1951,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>67</v>
       </c>
@@ -1969,7 +1968,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>67</v>
       </c>
@@ -1986,7 +1985,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>67</v>
       </c>
@@ -2003,7 +2002,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>68</v>
       </c>
@@ -2020,7 +2019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>68</v>
       </c>
@@ -2037,7 +2036,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>69</v>
       </c>
@@ -2054,7 +2053,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>69</v>
       </c>
@@ -2071,7 +2070,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>69</v>
       </c>
@@ -2088,7 +2087,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>69</v>
       </c>
@@ -2105,7 +2104,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>69</v>
       </c>
@@ -2122,7 +2121,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>72</v>
       </c>
@@ -2139,7 +2138,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>72</v>
       </c>
@@ -2156,7 +2155,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>72</v>
       </c>
@@ -2173,7 +2172,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>72</v>
       </c>
@@ -2190,7 +2189,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>74</v>
       </c>
@@ -2207,7 +2206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>74</v>
       </c>
@@ -2224,7 +2223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>74</v>
       </c>
@@ -2241,7 +2240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>74</v>
       </c>
@@ -2258,7 +2257,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>74</v>
       </c>
@@ -2275,7 +2274,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>76</v>
       </c>
@@ -2292,7 +2291,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>76</v>
       </c>
@@ -2309,7 +2308,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>76</v>
       </c>
@@ -2326,7 +2325,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>77</v>
       </c>
@@ -2343,7 +2342,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="38" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>77</v>
       </c>
@@ -2360,7 +2359,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>77</v>
       </c>
@@ -2377,7 +2376,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>77</v>
       </c>
@@ -2394,7 +2393,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="19" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
thêm data cho excel
</commit_message>
<xml_diff>
--- a/Tài liệu/chitietphancong_thuocbomon_CNTT.xlsx
+++ b/Tài liệu/chitietphancong_thuocbomon_CNTT.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="80">
   <si>
     <t>TENGV</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>Công nghệ phần mềm</t>
+  </si>
+  <si>
+    <t>THOIGIAN</t>
   </si>
 </sst>
 </file>
@@ -316,7 +319,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -339,11 +342,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -362,6 +376,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -677,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F103" sqref="F103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,10 +707,10 @@
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -709,8 +726,11 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F1" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -726,8 +746,11 @@
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -743,8 +766,11 @@
       <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -760,8 +786,11 @@
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -777,8 +806,11 @@
       <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -794,8 +826,11 @@
       <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -811,8 +846,11 @@
       <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -828,8 +866,11 @@
       <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -845,8 +886,11 @@
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -862,8 +906,11 @@
       <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -879,8 +926,11 @@
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -896,8 +946,11 @@
       <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
@@ -913,8 +966,11 @@
       <c r="E13" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
@@ -930,8 +986,11 @@
       <c r="E14" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
@@ -947,8 +1006,11 @@
       <c r="E15" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
@@ -964,8 +1026,11 @@
       <c r="E16" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
@@ -981,8 +1046,11 @@
       <c r="E17" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
@@ -998,8 +1066,11 @@
       <c r="E18" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>28</v>
       </c>
@@ -1015,8 +1086,11 @@
       <c r="E19" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>28</v>
       </c>
@@ -1032,8 +1106,11 @@
       <c r="E20" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>31</v>
       </c>
@@ -1049,8 +1126,11 @@
       <c r="E21" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>31</v>
       </c>
@@ -1066,8 +1146,11 @@
       <c r="E22" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>31</v>
       </c>
@@ -1083,8 +1166,11 @@
       <c r="E23" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>31</v>
       </c>
@@ -1100,8 +1186,11 @@
       <c r="E24" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
@@ -1117,8 +1206,11 @@
       <c r="E25" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>35</v>
       </c>
@@ -1134,8 +1226,11 @@
       <c r="E26" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>35</v>
       </c>
@@ -1151,8 +1246,11 @@
       <c r="E27" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>35</v>
       </c>
@@ -1168,8 +1266,11 @@
       <c r="E28" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
@@ -1185,42 +1286,51 @@
       <c r="E29" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>41</v>
+      <c r="B31" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>39</v>
       </c>
@@ -1228,7 +1338,7 @@
         <v>41</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>15</v>
@@ -1236,50 +1346,59 @@
       <c r="E32" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D34" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>32</v>
+      <c r="B35" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>8</v>
@@ -1287,33 +1406,39 @@
       <c r="E35" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>37</v>
+      <c r="B36" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>15</v>
@@ -1321,8 +1446,11 @@
       <c r="E37" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
@@ -1330,33 +1458,39 @@
         <v>43</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="D39" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="58.5" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -1364,7 +1498,7 @@
         <v>45</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>8</v>
@@ -1372,25 +1506,31 @@
       <c r="E40" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>46</v>
+      <c r="B41" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>44</v>
       </c>
@@ -1398,50 +1538,59 @@
         <v>46</v>
       </c>
       <c r="C42" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="D43" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>48</v>
+      <c r="B44" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>47</v>
       </c>
@@ -1449,33 +1598,39 @@
         <v>48</v>
       </c>
       <c r="C45" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="D46" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>49</v>
       </c>
@@ -1483,7 +1638,7 @@
         <v>50</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>8</v>
@@ -1491,25 +1646,31 @@
       <c r="E47" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>51</v>
+      <c r="B48" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>49</v>
       </c>
@@ -1517,7 +1678,7 @@
         <v>51</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>15</v>
@@ -1525,8 +1686,11 @@
       <c r="E49" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
@@ -1534,33 +1698,39 @@
         <v>51</v>
       </c>
       <c r="C50" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="D51" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>52</v>
       </c>
@@ -1568,7 +1738,7 @@
         <v>53</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>8</v>
@@ -1576,8 +1746,11 @@
       <c r="E52" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
@@ -1585,7 +1758,7 @@
         <v>53</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>8</v>
@@ -1593,8 +1766,11 @@
       <c r="E53" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
@@ -1602,7 +1778,7 @@
         <v>53</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>8</v>
@@ -1610,16 +1786,19 @@
       <c r="E54" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>8</v>
@@ -1627,25 +1806,31 @@
       <c r="E55" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>55</v>
+      <c r="B56" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>52</v>
       </c>
@@ -1653,33 +1838,39 @@
         <v>55</v>
       </c>
       <c r="C57" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="39" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D58" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
@@ -1687,41 +1878,47 @@
         <v>58</v>
       </c>
       <c r="C59" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="D60" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>7</v>
+      <c r="C61" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>8</v>
@@ -1729,25 +1926,31 @@
       <c r="E61" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>61</v>
+      <c r="B62" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>60</v>
       </c>
@@ -1755,7 +1958,7 @@
         <v>61</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>15</v>
@@ -1763,42 +1966,51 @@
       <c r="E63" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C65" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="D65" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>62</v>
       </c>
@@ -1806,7 +2018,7 @@
         <v>63</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>8</v>
@@ -1814,42 +2026,51 @@
       <c r="E66" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B67" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B68" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C68" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="39" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="D68" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>65</v>
       </c>
@@ -1857,7 +2078,7 @@
         <v>58</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>8</v>
@@ -1865,76 +2086,91 @@
       <c r="E69" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B71" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C71" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="D71" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B73" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C73" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="D73" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>67</v>
       </c>
@@ -1942,7 +2178,7 @@
         <v>63</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>8</v>
@@ -1950,33 +2186,39 @@
       <c r="E74" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B75" s="3" t="s">
-        <v>41</v>
+      <c r="B75" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>15</v>
@@ -1984,8 +2226,11 @@
       <c r="E76" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>67</v>
       </c>
@@ -1993,33 +2238,39 @@
         <v>61</v>
       </c>
       <c r="C77" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C78" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="D78" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F78">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>68</v>
       </c>
@@ -2027,50 +2278,59 @@
         <v>46</v>
       </c>
       <c r="C79" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C80" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="D80" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B81" s="3" t="s">
-        <v>71</v>
+      <c r="B81" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F81">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>69</v>
       </c>
@@ -2078,7 +2338,7 @@
         <v>71</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>15</v>
@@ -2086,16 +2346,19 @@
       <c r="E82" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>15</v>
@@ -2103,8 +2366,11 @@
       <c r="E83" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F83">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>69</v>
       </c>
@@ -2112,33 +2378,39 @@
         <v>38</v>
       </c>
       <c r="C84" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C85" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D84" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="D85" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F85">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>72</v>
       </c>
@@ -2146,7 +2418,7 @@
         <v>70</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>8</v>
@@ -2154,25 +2426,31 @@
       <c r="E86" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F86">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B87" s="3" t="s">
-        <v>73</v>
+      <c r="B87" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F87">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>72</v>
       </c>
@@ -2180,33 +2458,39 @@
         <v>73</v>
       </c>
       <c r="C88" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F88">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="D89" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F89">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>74</v>
       </c>
@@ -2214,7 +2498,7 @@
         <v>50</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>8</v>
@@ -2222,25 +2506,31 @@
       <c r="E90" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F90">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B91" s="3" t="s">
-        <v>75</v>
+      <c r="B91" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>74</v>
       </c>
@@ -2248,7 +2538,7 @@
         <v>75</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>15</v>
@@ -2256,8 +2546,11 @@
       <c r="E92" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F92">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>74</v>
       </c>
@@ -2265,33 +2558,39 @@
         <v>75</v>
       </c>
       <c r="C93" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F93">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C94" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D93" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="39" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="D94" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F94">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>76</v>
       </c>
@@ -2299,7 +2598,7 @@
         <v>32</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>8</v>
@@ -2307,42 +2606,51 @@
       <c r="E95" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F95">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B96" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F96">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B97" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="39" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F97">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>77</v>
       </c>
@@ -2350,7 +2658,7 @@
         <v>54</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>8</v>
@@ -2358,25 +2666,31 @@
       <c r="E98" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F98">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B99" s="3" t="s">
-        <v>78</v>
+      <c r="B99" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F99">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>77</v>
       </c>
@@ -2384,7 +2698,7 @@
         <v>78</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>15</v>
@@ -2392,8 +2706,11 @@
       <c r="E100" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F100">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>77</v>
       </c>
@@ -2401,13 +2718,36 @@
         <v>78</v>
       </c>
       <c r="C101" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F101">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C102" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D101" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>9</v>
+      <c r="D102" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F102">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>